<commit_message>
Fixed missing tag on institutions
</commit_message>
<xml_diff>
--- a/inst/extdata/institution_strings.xlsx
+++ b/inst/extdata/institution_strings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenjitomari/Documents/GitHub/dope1/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3269CE03-715B-2241-A923-BF4E8D5B8652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC86FF72-4DA9-5842-9911-0F7E7A15D834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="1120" windowWidth="29080" windowHeight="17260" activeTab="1" xr2:uid="{E96A2A2D-4572-B745-B015-D596C354435F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="824">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="824">
   <si>
     <t>Israel Institute of Technology</t>
   </si>
@@ -3304,8 +3304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DEBFD4E-337F-8B41-884F-DB9881B17140}">
   <dimension ref="A1:F235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
-      <selection activeCell="B242" sqref="B242"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D125" sqref="D125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5196,7 +5196,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>532</v>
       </c>
@@ -5207,7 +5207,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>535</v>
       </c>
@@ -5218,7 +5218,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>538</v>
       </c>
@@ -5229,7 +5229,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>541</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>541</v>
       </c>
@@ -5254,7 +5254,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>544</v>
       </c>
@@ -5265,7 +5265,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>544</v>
       </c>
@@ -5279,7 +5279,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>548</v>
       </c>
@@ -5289,8 +5289,11 @@
       <c r="C152" s="1" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E152" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>551</v>
       </c>
@@ -5304,7 +5307,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>555</v>
       </c>
@@ -5318,7 +5321,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>559</v>
       </c>
@@ -5329,7 +5332,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>562</v>
       </c>
@@ -5343,7 +5346,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>566</v>
       </c>
@@ -5357,7 +5360,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>570</v>
       </c>
@@ -5371,7 +5374,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>574</v>
       </c>
@@ -5382,7 +5385,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>577</v>
       </c>

</xml_diff>